<commit_message>
template transaksi user update
</commit_message>
<xml_diff>
--- a/public/template-excel/template-transaksiuser.xlsx
+++ b/public/template-excel/template-transaksiuser.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WinNMP\WWW\simpinlaravel\simpin\public\template-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E6BC66-FD60-4D05-96D7-D37A48E070BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038DDD8D-4B81-416F-921F-150FE5930ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$W$4</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$R$1:$V$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$Y$4</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$T$1:$X$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>NAMA</t>
   </si>
@@ -122,6 +122,18 @@
   </si>
   <si>
     <t>KETERANGAN</t>
+  </si>
+  <si>
+    <t>106.02.060</t>
+  </si>
+  <si>
+    <t>KODE_PINJAM1</t>
+  </si>
+  <si>
+    <t>KODE_PINJAM2</t>
+  </si>
+  <si>
+    <t>10602060-2985-12032021165439</t>
   </si>
 </sst>
 </file>
@@ -823,676 +835,683 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:AA25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" style="30" customWidth="1"/>
-    <col min="2" max="2" width="3.42578125" style="31" customWidth="1"/>
-    <col min="3" max="3" width="11" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="19" customWidth="1"/>
-    <col min="7" max="8" width="11.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" style="19" customWidth="1"/>
-    <col min="11" max="11" width="10" style="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3" style="31" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3" style="31" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.140625" style="47" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8" style="46" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" style="5" customWidth="1"/>
-    <col min="18" max="18" width="5.140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.42578125" style="55" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.140625" style="51" customWidth="1"/>
-    <col min="22" max="22" width="28.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.85546875" style="68" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="28.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" style="30" customWidth="1"/>
+    <col min="4" max="4" width="3.42578125" style="31" customWidth="1"/>
+    <col min="5" max="5" width="11" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="19" customWidth="1"/>
+    <col min="9" max="10" width="11.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" style="19" customWidth="1"/>
+    <col min="13" max="13" width="10" style="19" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3" style="31" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3" style="31" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8" style="46" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" style="5" customWidth="1"/>
+    <col min="20" max="20" width="5.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.42578125" style="55" customWidth="1"/>
+    <col min="22" max="22" width="9.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.140625" style="51" customWidth="1"/>
+    <col min="24" max="24" width="28.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.85546875" style="68" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:27" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="D1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="G1" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="H1" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="I1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="J1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="K1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="L1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="M1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="N1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="O1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="37" t="s">
+      <c r="P1" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="38" t="s">
+      <c r="Q1" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="R1" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="40" t="s">
+      <c r="T1" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="52" t="s">
+      <c r="U1" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="T1" s="48" t="s">
+      <c r="V1" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="49" t="s">
+      <c r="W1" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V1" s="17" t="s">
+      <c r="X1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="X1" s="67" t="s">
+      <c r="Z1" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="AA1" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28">
+    <row r="2" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="28">
         <v>2021</v>
       </c>
-      <c r="B2" s="29">
+      <c r="D2" s="29">
         <v>5</v>
       </c>
-      <c r="C2" s="56">
+      <c r="E2" s="56">
         <v>271108276</v>
       </c>
-      <c r="D2" s="11">
-        <v>10602060</v>
-      </c>
-      <c r="E2" s="33">
-        <v>10602060</v>
-      </c>
-      <c r="F2" s="57">
+      <c r="F2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="57">
         <v>1000000</v>
       </c>
-      <c r="G2" s="57">
+      <c r="I2" s="57">
         <v>500000</v>
       </c>
-      <c r="H2" s="15">
+      <c r="J2" s="15">
         <v>500000000</v>
       </c>
-      <c r="I2" s="14">
+      <c r="K2" s="14">
         <v>60</v>
       </c>
-      <c r="J2" s="57">
+      <c r="L2" s="57">
         <v>8333334</v>
       </c>
-      <c r="K2" s="57">
+      <c r="M2" s="57">
         <v>5000000</v>
       </c>
-      <c r="L2" s="29">
+      <c r="N2" s="29">
         <v>0</v>
       </c>
-      <c r="M2" s="29"/>
-      <c r="N2" s="58">
+      <c r="O2" s="29"/>
+      <c r="P2" s="58">
         <v>0</v>
       </c>
-      <c r="O2" s="58">
+      <c r="Q2" s="58">
         <v>0</v>
       </c>
-      <c r="P2" s="41">
+      <c r="R2" s="41">
         <v>0</v>
       </c>
-      <c r="Q2" s="8">
-        <f>F2+G2+J2+K2+N2+O2</f>
+      <c r="S2" s="8">
         <v>14833334</v>
       </c>
-      <c r="R2" s="42">
+      <c r="T2" s="42">
         <v>1</v>
       </c>
-      <c r="S2" s="59">
+      <c r="U2" s="59">
         <v>2985</v>
       </c>
-      <c r="T2" s="60">
+      <c r="V2" s="60">
         <v>18</v>
       </c>
-      <c r="U2" s="61" t="s">
+      <c r="W2" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="V2" s="62" t="s">
+      <c r="X2" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="9" t="s">
+      <c r="Y2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="X2" s="67">
-        <v>44440</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28">
+      <c r="Z2" s="67">
+        <v>44805</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="28">
         <v>2021</v>
       </c>
-      <c r="B3" s="29">
+      <c r="D3" s="29">
         <v>5</v>
       </c>
-      <c r="C3" s="56">
+      <c r="E3" s="56">
         <v>268068822</v>
       </c>
-      <c r="D3" s="11">
-        <v>10602060</v>
-      </c>
-      <c r="E3" s="33">
-        <v>10602060</v>
-      </c>
-      <c r="F3" s="57">
+      <c r="F3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="57">
         <v>100000</v>
       </c>
-      <c r="G3" s="57">
+      <c r="I3" s="57">
         <v>0</v>
       </c>
-      <c r="H3" s="15">
+      <c r="J3" s="15">
         <v>497000000</v>
       </c>
-      <c r="I3" s="14">
+      <c r="K3" s="14">
         <v>60</v>
       </c>
-      <c r="J3" s="57">
+      <c r="L3" s="57">
         <v>8283334</v>
       </c>
-      <c r="K3" s="57">
+      <c r="M3" s="57">
         <v>4970000</v>
       </c>
-      <c r="L3" s="29">
+      <c r="N3" s="29">
         <v>0</v>
       </c>
-      <c r="M3" s="29"/>
-      <c r="N3" s="58">
+      <c r="O3" s="29"/>
+      <c r="P3" s="58">
         <v>0</v>
       </c>
-      <c r="O3" s="58">
+      <c r="Q3" s="58">
         <v>0</v>
       </c>
-      <c r="P3" s="41">
+      <c r="R3" s="41">
         <v>0</v>
       </c>
-      <c r="Q3" s="8">
-        <f>F3+G3+J3+K3+N3+O3</f>
+      <c r="S3" s="8">
         <v>13353334</v>
       </c>
-      <c r="R3" s="42">
+      <c r="T3" s="42">
         <v>2</v>
       </c>
-      <c r="S3" s="59">
+      <c r="U3" s="59">
         <v>4154</v>
       </c>
-      <c r="T3" s="60">
+      <c r="V3" s="60">
         <v>18</v>
       </c>
-      <c r="U3" s="61" t="s">
+      <c r="W3" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="V3" s="62" t="s">
+      <c r="X3" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="W3" s="9" t="s">
+      <c r="Y3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="X3" s="67">
-        <v>44440</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="63"/>
-      <c r="K4" s="63"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="64"/>
-      <c r="O4" s="64"/>
-      <c r="P4" s="41"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="42">
+      <c r="Z3" s="67">
+        <v>44805</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="28"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="64"/>
+      <c r="Q4" s="64"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="42">
         <v>295</v>
       </c>
-      <c r="S4" s="54"/>
-      <c r="T4" s="65"/>
-      <c r="U4" s="66"/>
-      <c r="V4" s="24"/>
-      <c r="X4" s="67"/>
-    </row>
-    <row r="5" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
+      <c r="U4" s="54"/>
+      <c r="V4" s="65"/>
+      <c r="W4" s="66"/>
+      <c r="X4" s="24"/>
+      <c r="Z4" s="67"/>
+    </row>
+    <row r="5" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="28"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="34"/>
       <c r="H5" s="15"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="53"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="50"/>
-      <c r="V5" s="13"/>
-      <c r="X5" s="67"/>
-    </row>
-    <row r="6" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="28"/>
+      <c r="U5" s="53"/>
+      <c r="V5" s="29"/>
+      <c r="W5" s="50"/>
+      <c r="X5" s="13"/>
+      <c r="Z5" s="67"/>
+    </row>
+    <row r="6" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="28"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="34"/>
       <c r="H6" s="15"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="44"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
-      <c r="P6" s="41"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="28"/>
-      <c r="S6" s="53"/>
-      <c r="T6" s="29"/>
-      <c r="U6" s="50"/>
-      <c r="V6" s="13"/>
-      <c r="X6" s="67"/>
-    </row>
-    <row r="7" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="45"/>
+      <c r="R6" s="41"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="28"/>
+      <c r="U6" s="53"/>
+      <c r="V6" s="29"/>
+      <c r="W6" s="50"/>
+      <c r="X6" s="13"/>
+      <c r="Z6" s="67"/>
+    </row>
+    <row r="7" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="28"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="15"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="44"/>
-      <c r="M7" s="44"/>
-      <c r="N7" s="45"/>
-      <c r="O7" s="45"/>
-      <c r="P7" s="41"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="28"/>
-      <c r="S7" s="53"/>
-      <c r="T7" s="29"/>
-      <c r="U7" s="50"/>
-      <c r="V7" s="13"/>
-      <c r="X7" s="67"/>
-    </row>
-    <row r="8" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="45"/>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="41"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="28"/>
+      <c r="U7" s="53"/>
+      <c r="V7" s="29"/>
+      <c r="W7" s="50"/>
+      <c r="X7" s="13"/>
+      <c r="Z7" s="67"/>
+    </row>
+    <row r="8" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="28"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="34"/>
       <c r="H8" s="15"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="44"/>
-      <c r="M8" s="44"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="45"/>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="28"/>
-      <c r="S8" s="53"/>
-      <c r="T8" s="29"/>
-      <c r="U8" s="50"/>
-      <c r="V8" s="13"/>
-      <c r="X8" s="67"/>
-    </row>
-    <row r="9" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="45"/>
+      <c r="Q8" s="45"/>
+      <c r="R8" s="41"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="28"/>
+      <c r="U8" s="53"/>
+      <c r="V8" s="29"/>
+      <c r="W8" s="50"/>
+      <c r="X8" s="13"/>
+      <c r="Z8" s="67"/>
+    </row>
+    <row r="9" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="28"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="34"/>
       <c r="H9" s="15"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="44"/>
-      <c r="N9" s="45"/>
-      <c r="O9" s="45"/>
-      <c r="P9" s="41"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="28"/>
-      <c r="S9" s="53"/>
-      <c r="T9" s="29"/>
-      <c r="U9" s="50"/>
-      <c r="V9" s="13"/>
-      <c r="X9" s="67"/>
-    </row>
-    <row r="10" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="44"/>
+      <c r="O9" s="44"/>
+      <c r="P9" s="45"/>
+      <c r="Q9" s="45"/>
+      <c r="R9" s="41"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="28"/>
+      <c r="U9" s="53"/>
+      <c r="V9" s="29"/>
+      <c r="W9" s="50"/>
+      <c r="X9" s="13"/>
+      <c r="Z9" s="67"/>
+    </row>
+    <row r="10" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="28"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="34"/>
       <c r="H10" s="15"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="45"/>
-      <c r="O10" s="45"/>
-      <c r="P10" s="41"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="28"/>
-      <c r="S10" s="53"/>
-      <c r="T10" s="29"/>
-      <c r="U10" s="50"/>
-      <c r="V10" s="13"/>
-      <c r="X10" s="67"/>
-    </row>
-    <row r="11" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="45"/>
+      <c r="Q10" s="45"/>
+      <c r="R10" s="41"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="28"/>
+      <c r="U10" s="53"/>
+      <c r="V10" s="29"/>
+      <c r="W10" s="50"/>
+      <c r="X10" s="13"/>
+      <c r="Z10" s="67"/>
+    </row>
+    <row r="11" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="28"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="34"/>
       <c r="H11" s="15"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="44"/>
-      <c r="N11" s="45"/>
-      <c r="O11" s="45"/>
-      <c r="P11" s="41"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="28"/>
-      <c r="S11" s="53"/>
-      <c r="T11" s="29"/>
-      <c r="U11" s="50"/>
-      <c r="V11" s="13"/>
-      <c r="X11" s="67"/>
-    </row>
-    <row r="12" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="45"/>
+      <c r="R11" s="41"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="28"/>
+      <c r="U11" s="53"/>
+      <c r="V11" s="29"/>
+      <c r="W11" s="50"/>
+      <c r="X11" s="13"/>
+      <c r="Z11" s="67"/>
+    </row>
+    <row r="12" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="28"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="33"/>
       <c r="H12" s="15"/>
-      <c r="I12" s="14"/>
+      <c r="I12" s="15"/>
       <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="43"/>
-      <c r="P12" s="41"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="28"/>
-      <c r="S12" s="53"/>
-      <c r="T12" s="29"/>
-      <c r="U12" s="50"/>
-      <c r="V12" s="13"/>
-      <c r="X12" s="67"/>
-    </row>
-    <row r="13" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="41"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="28"/>
+      <c r="U12" s="53"/>
+      <c r="V12" s="29"/>
+      <c r="W12" s="50"/>
+      <c r="X12" s="13"/>
+      <c r="Z12" s="67"/>
+    </row>
+    <row r="13" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="28"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="33"/>
       <c r="H13" s="15"/>
-      <c r="I13" s="14"/>
+      <c r="I13" s="15"/>
       <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="43"/>
-      <c r="O13" s="43"/>
-      <c r="P13" s="41"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="28"/>
-      <c r="S13" s="53"/>
-      <c r="T13" s="29"/>
-      <c r="U13" s="50"/>
-      <c r="V13" s="13"/>
-      <c r="X13" s="67"/>
-    </row>
-    <row r="14" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="43"/>
+      <c r="R13" s="41"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="28"/>
+      <c r="U13" s="53"/>
+      <c r="V13" s="29"/>
+      <c r="W13" s="50"/>
+      <c r="X13" s="13"/>
+      <c r="Z13" s="67"/>
+    </row>
+    <row r="14" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="28"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="33"/>
       <c r="H14" s="15"/>
-      <c r="I14" s="14"/>
+      <c r="I14" s="15"/>
       <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="43"/>
-      <c r="O14" s="43"/>
-      <c r="P14" s="41"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="28"/>
-      <c r="S14" s="53"/>
-      <c r="T14" s="29"/>
-      <c r="U14" s="50"/>
-      <c r="V14" s="13"/>
-      <c r="X14" s="67"/>
-    </row>
-    <row r="15" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="41"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="28"/>
+      <c r="U14" s="53"/>
+      <c r="V14" s="29"/>
+      <c r="W14" s="50"/>
+      <c r="X14" s="13"/>
+      <c r="Z14" s="67"/>
+    </row>
+    <row r="15" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="28"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="33"/>
       <c r="H15" s="15"/>
-      <c r="I15" s="14"/>
+      <c r="I15" s="15"/>
       <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="43"/>
-      <c r="O15" s="43"/>
-      <c r="P15" s="41"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="28"/>
-      <c r="S15" s="53"/>
-      <c r="T15" s="29"/>
-      <c r="U15" s="50"/>
-      <c r="V15" s="13"/>
-      <c r="X15" s="67"/>
-    </row>
-    <row r="16" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="43"/>
+      <c r="Q15" s="43"/>
+      <c r="R15" s="41"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="28"/>
+      <c r="U15" s="53"/>
+      <c r="V15" s="29"/>
+      <c r="W15" s="50"/>
+      <c r="X15" s="13"/>
+      <c r="Z15" s="67"/>
+    </row>
+    <row r="16" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="28"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="33"/>
       <c r="H16" s="15"/>
-      <c r="I16" s="14"/>
+      <c r="I16" s="15"/>
       <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="43"/>
-      <c r="O16" s="43"/>
-      <c r="P16" s="41"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="28"/>
-      <c r="S16" s="53"/>
-      <c r="T16" s="29"/>
-      <c r="U16" s="50"/>
-      <c r="V16" s="13"/>
-      <c r="X16" s="67"/>
-    </row>
-    <row r="17" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="29"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="43"/>
+      <c r="Q16" s="43"/>
+      <c r="R16" s="41"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="28"/>
+      <c r="U16" s="53"/>
+      <c r="V16" s="29"/>
+      <c r="W16" s="50"/>
+      <c r="X16" s="13"/>
+      <c r="Z16" s="67"/>
+    </row>
+    <row r="17" spans="3:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="33"/>
       <c r="H17" s="15"/>
-      <c r="I17" s="14"/>
+      <c r="I17" s="15"/>
       <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="43"/>
-      <c r="O17" s="43"/>
-      <c r="P17" s="41"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="28"/>
-      <c r="S17" s="53"/>
-      <c r="T17" s="29"/>
-      <c r="U17" s="50"/>
-      <c r="V17" s="13"/>
-      <c r="X17" s="67"/>
-    </row>
-    <row r="18" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="43"/>
+      <c r="Q17" s="43"/>
+      <c r="R17" s="41"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="28"/>
+      <c r="U17" s="53"/>
+      <c r="V17" s="29"/>
+      <c r="W17" s="50"/>
+      <c r="X17" s="13"/>
+      <c r="Z17" s="67"/>
+    </row>
+    <row r="18" spans="3:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="28"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="33"/>
       <c r="H18" s="15"/>
-      <c r="I18" s="14"/>
+      <c r="I18" s="15"/>
       <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="43"/>
-      <c r="O18" s="43"/>
-      <c r="P18" s="41"/>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="28"/>
-      <c r="S18" s="53"/>
-      <c r="T18" s="29"/>
-      <c r="U18" s="50"/>
-      <c r="V18" s="13"/>
-      <c r="X18" s="67"/>
-    </row>
-    <row r="19" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="43"/>
+      <c r="Q18" s="43"/>
+      <c r="R18" s="41"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="28"/>
+      <c r="U18" s="53"/>
+      <c r="V18" s="29"/>
+      <c r="W18" s="50"/>
+      <c r="X18" s="13"/>
+      <c r="Z18" s="67"/>
+    </row>
+    <row r="19" spans="3:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="28"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="33"/>
       <c r="H19" s="15"/>
-      <c r="I19" s="14"/>
+      <c r="I19" s="15"/>
       <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="43"/>
-      <c r="O19" s="43"/>
-      <c r="P19" s="41"/>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="28"/>
-      <c r="S19" s="53"/>
-      <c r="T19" s="29"/>
-      <c r="U19" s="50"/>
-      <c r="V19" s="13"/>
-      <c r="X19" s="67"/>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B20" s="29"/>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B21" s="29"/>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="29"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="43"/>
+      <c r="Q19" s="43"/>
+      <c r="R19" s="41"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="28"/>
+      <c r="U19" s="53"/>
+      <c r="V19" s="29"/>
+      <c r="W19" s="50"/>
+      <c r="X19" s="13"/>
+      <c r="Z19" s="67"/>
+    </row>
+    <row r="20" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="D20" s="29"/>
+    </row>
+    <row r="21" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="D21" s="29"/>
+    </row>
+    <row r="22" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="D22" s="29"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -1511,12 +1530,12 @@
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="29"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+    </row>
+    <row r="23" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="D23" s="29"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -1535,12 +1554,12 @@
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="29"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+    </row>
+    <row r="24" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="D24" s="29"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1559,12 +1578,12 @@
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="29"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+    </row>
+    <row r="25" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="D25" s="29"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1583,10 +1602,12 @@
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W3">
-    <sortCondition descending="1" ref="Q2:Q3"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:Y3">
+    <sortCondition descending="1" ref="S2:S3"/>
   </sortState>
   <pageMargins left="0.78" right="0.70866141732283472" top="1.41" bottom="3.937007874015748E-2" header="0.73" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="landscape" r:id="rId1"/>

</xml_diff>